<commit_message>
Added original translation image files
</commit_message>
<xml_diff>
--- a/Una deformación de la realidad/Imágenes - Una deformación de la realidad.xlsx
+++ b/Una deformación de la realidad/Imágenes - Una deformación de la realidad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Valk\Valkyrie-Mom-scenarios-translations\Una deformación de la realidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F568532D-283F-429B-A0B3-D56A38D74EED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B2BA01-24B8-4B21-90BD-1944B0EE60EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -608,14 +608,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -646,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -660,7 +660,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="105" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -672,7 +672,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -896,8 +908,8 @@
   <dimension ref="A1:D1188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="70.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -921,226 +933,226 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="204" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:4" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:4" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:4" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:4" ht="165.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:4" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:4" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="153" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="10" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:4" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="3"/>
@@ -1164,13 +1176,13 @@
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:4" ht="191.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -1178,158 +1190,158 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="11"/>
     </row>
     <row r="31" spans="1:4" ht="293.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="191.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="11" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="10" t="s">
         <v>69</v>
       </c>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="10" t="s">
         <v>73</v>
       </c>
       <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="10" t="s">
         <v>75</v>
       </c>
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="10" t="s">
         <v>77</v>
       </c>
       <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="10" t="s">
         <v>79</v>
       </c>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="10" t="s">
         <v>81</v>
       </c>
       <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="3"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="10" t="s">
         <v>87</v>
       </c>
       <c r="C44" s="3"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="10" t="s">
         <v>89</v>
       </c>
       <c r="C45" s="3"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="10" t="s">
         <v>91</v>
       </c>
       <c r="C46" s="3"/>
@@ -1360,88 +1372,88 @@
       <c r="C49" s="3"/>
     </row>
     <row r="50" spans="1:3" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="9" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="204" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="9" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C52" s="3"/>
+      <c r="C52" s="9"/>
     </row>
     <row r="53" spans="1:3" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="9" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="9" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="9" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="9" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="9" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated translation files for Strain on Reality Spanish
</commit_message>
<xml_diff>
--- a/Una deformación de la realidad/Imágenes - Una deformación de la realidad.xlsx
+++ b/Una deformación de la realidad/Imágenes - Una deformación de la realidad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Valk\Valkyrie-Mom-scenarios-translations\Una deformación de la realidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B2BA01-24B8-4B21-90BD-1944B0EE60EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C1E3BF-A3DB-481E-A91D-DA71D79D72D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -908,8 +908,8 @@
   <dimension ref="A1:D1188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="70.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1158,19 +1158,19 @@
       <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:4" ht="293.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="10" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:4" ht="280.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="10" t="s">
         <v>51</v>
       </c>
       <c r="C28" s="3"/>
@@ -1347,19 +1347,19 @@
       <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:3" ht="191.25" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="10" t="s">
         <v>93</v>
       </c>
       <c r="C47" s="3"/>
     </row>
     <row r="48" spans="1:3" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="10" t="s">
         <v>95</v>
       </c>
       <c r="C48" s="3"/>

</xml_diff>

<commit_message>
All but two images updated
</commit_message>
<xml_diff>
--- a/Una deformación de la realidad/Imágenes - Una deformación de la realidad.xlsx
+++ b/Una deformación de la realidad/Imágenes - Una deformación de la realidad.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Valk\Valkyrie-Mom-scenarios-translations\Una deformación de la realidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C1E3BF-A3DB-481E-A91D-DA71D79D72D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FE848D-7E1B-4E1B-A3C8-C3DA630D7FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -565,7 +565,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -591,6 +591,12 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -646,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -685,6 +691,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -908,8 +917,8 @@
   <dimension ref="A1:D1188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48:B48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="70.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1467,57 +1476,57 @@
       <c r="C58" s="3"/>
     </row>
     <row r="59" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C59" s="3"/>
     </row>
     <row r="60" spans="1:3" ht="204" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="9" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="10" t="s">
         <v>128</v>
       </c>
       <c r="C61" s="3"/>
     </row>
     <row r="62" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="10" t="s">
         <v>130</v>
       </c>
       <c r="C62" s="3"/>
     </row>
     <row r="63" spans="1:3" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="14" t="s">
         <v>132</v>
       </c>
       <c r="C63" s="3"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="14" t="s">
         <v>134</v>
       </c>
       <c r="C64" s="3"/>

</xml_diff>